<commit_message>
Modifications ref et grilles STS SN
</commit_message>
<xml_diff>
--- a/tables/Grille BTS SN EC_Sit1.xlsx
+++ b/tables/Grille BTS SN EC_Sit1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="-15" windowWidth="10710" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="10905" yWindow="-15" windowWidth="10710" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Identification projet" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Identification projet'!$A$1:$B$57</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Notation Sit1 candidat 1'!$A$1:$K$37</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>Identifications</t>
   </si>
@@ -114,15 +114,6 @@
   </si>
   <si>
     <t>non</t>
-  </si>
-  <si>
-    <t>1/3</t>
-  </si>
-  <si>
-    <t>2/3</t>
-  </si>
-  <si>
-    <t>3/3</t>
   </si>
   <si>
     <t>éval</t>
@@ -329,11 +320,26 @@
   <si>
     <t>Le matériel est préparé pour mettre en œuvre la solution.</t>
   </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -595,7 +601,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="68">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -1441,6 +1447,67 @@
       <top/>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1496,7 +1563,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1826,11 +1893,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1847,48 +1957,59 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1909,29 +2030,64 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1945,136 +2101,93 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2128,7 +2241,20 @@
     <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
@@ -2208,17 +2334,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -2229,14 +2345,13 @@
           <c:yMode val="edge"/>
           <c:x val="7.3170441237768197E-2"/>
           <c:y val="4.9689440993788803E-2"/>
-          <c:w val="0.86178519680038101"/>
-          <c:h val="0.92546583850931696"/>
+          <c:w val="0.86178519680038113"/>
+          <c:h val="0.92546583850931707"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2251,7 +2366,6 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'Notation Sit1 candidat 1'!$T$6:$T$9</c:f>
@@ -2259,10 +2373,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2274,20 +2388,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="75399936"/>
-        <c:axId val="75401472"/>
+        <c:dLbls/>
+        <c:axId val="129707008"/>
+        <c:axId val="129712896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75399936"/>
+        <c:axId val="129707008"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2303,18 +2409,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75401472"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129712896"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75401472"/>
+        <c:axId val="129712896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2323,13 +2426,11 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75399936"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129707008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33329999999999999"/>
+        <c:majorUnit val="0.3333000000000001"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2343,7 +2444,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2370,7 +2470,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555607" footer="0.51180555555555607"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2378,17 +2478,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -2398,15 +2488,14 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="7.3770713242967703E-2"/>
-          <c:y val="3.7558599346667401E-2"/>
-          <c:w val="0.86885506708384097"/>
-          <c:h val="0.93427015874835195"/>
+          <c:y val="3.7558599346667394E-2"/>
+          <c:w val="0.86885506708384119"/>
+          <c:h val="0.93427015874835184"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2421,7 +2510,6 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'Notation candidat 1'!#REF!</c:f>
@@ -2435,20 +2523,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="75421184"/>
-        <c:axId val="75422720"/>
+        <c:dLbls/>
+        <c:axId val="129748992"/>
+        <c:axId val="129750528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75421184"/>
+        <c:axId val="129748992"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2464,18 +2544,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75422720"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129750528"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75422720"/>
+        <c:axId val="129750528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2484,13 +2561,11 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75421184"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129748992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33329999999999999"/>
+        <c:majorUnit val="0.3333000000000001"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2504,7 +2579,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2531,7 +2605,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555607" footer="0.51180555555555607"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2539,17 +2613,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -2560,14 +2624,13 @@
           <c:yMode val="edge"/>
           <c:x val="7.3170441237768197E-2"/>
           <c:y val="4.9689440993788803E-2"/>
-          <c:w val="0.86178519680038101"/>
-          <c:h val="0.92546583850931696"/>
+          <c:w val="0.86178519680038113"/>
+          <c:h val="0.92546583850931707"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2582,7 +2645,6 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'Notation Sit1 candidat 1'!$T$16:$T$19</c:f>
@@ -2605,20 +2667,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="80902400"/>
-        <c:axId val="80904192"/>
+        <c:dLbls/>
+        <c:axId val="129778432"/>
+        <c:axId val="129779968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80902400"/>
+        <c:axId val="129778432"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2634,18 +2688,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80904192"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129779968"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80904192"/>
+        <c:axId val="129779968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2654,13 +2705,11 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80902400"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129778432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33329999999999999"/>
+        <c:majorUnit val="0.3333000000000001"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2674,7 +2723,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2701,7 +2749,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555607" footer="0.51180555555555607"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2709,17 +2757,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -2730,14 +2768,13 @@
           <c:yMode val="edge"/>
           <c:x val="7.3170441237768197E-2"/>
           <c:y val="4.9689440993788803E-2"/>
-          <c:w val="0.86178519680038101"/>
-          <c:h val="0.92546583850931696"/>
+          <c:w val="0.86178519680038113"/>
+          <c:h val="0.92546583850931707"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2752,7 +2789,6 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'Notation Sit1 candidat 1'!$T$11:$T$14</c:f>
@@ -2775,20 +2811,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="81285120"/>
-        <c:axId val="81286656"/>
+        <c:dLbls/>
+        <c:axId val="129811968"/>
+        <c:axId val="129813504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81285120"/>
+        <c:axId val="129811968"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2804,18 +2832,15 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81286656"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129813504"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81286656"/>
+        <c:axId val="129813504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2824,13 +2849,11 @@
         <c:delete val="1"/>
         <c:axPos val="t"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81285120"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="129811968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.33329999999999999"/>
+        <c:majorUnit val="0.3333000000000001"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2844,7 +2867,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:noFill/>
@@ -2871,7 +2893,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555607" footer="0.51180555555555607"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2916,7 +2938,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2926,7 +2948,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2986,7 +3008,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2996,7 +3018,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3124,12 +3146,12 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3511,11 +3533,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -3525,7 +3547,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3555,11 +3577,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -3569,7 +3591,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -3590,14 +3612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -3609,25 +3631,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" customHeight="1">
-      <c r="A1" s="107" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="107"/>
+      <c r="A1" s="124" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="124"/>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="138" t="s">
-        <v>64</v>
+      <c r="B3" s="106" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3635,7 +3657,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3671,10 +3693,10 @@
       <c r="B9" s="10"/>
     </row>
     <row r="10" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="106"/>
+      <c r="B10" s="125"/>
     </row>
     <row r="11" spans="1:2" ht="18.2" customHeight="1">
       <c r="A11" s="5" t="s">
@@ -3689,10 +3711,10 @@
       <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A13" s="106" t="s">
+      <c r="A13" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="106"/>
+      <c r="B13" s="125"/>
     </row>
     <row r="14" spans="1:2" ht="18.2" customHeight="1">
       <c r="A14" s="5" t="s">
@@ -3707,10 +3729,10 @@
       <c r="B15" s="11"/>
     </row>
     <row r="16" spans="1:2" ht="12.75" customHeight="1">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="125" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="106"/>
+      <c r="B16" s="125"/>
     </row>
     <row r="17" spans="1:3" ht="18.2" customHeight="1">
       <c r="A17" s="5" t="s">
@@ -3725,10 +3747,10 @@
       <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A19" s="106" t="s">
+      <c r="A19" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="106"/>
+      <c r="B19" s="125"/>
     </row>
     <row r="20" spans="1:3" ht="18.2" customHeight="1">
       <c r="A20" s="5" t="s">
@@ -3743,96 +3765,96 @@
       <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A22" s="108" t="s">
+      <c r="A22" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="108"/>
+      <c r="B22" s="120"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="110"/>
-      <c r="B23" s="110"/>
+      <c r="A23" s="122"/>
+      <c r="B23" s="122"/>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A24" s="110"/>
-      <c r="B24" s="110"/>
+      <c r="A24" s="122"/>
+      <c r="B24" s="122"/>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A25" s="110"/>
-      <c r="B25" s="110"/>
+      <c r="A25" s="122"/>
+      <c r="B25" s="122"/>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A26" s="110"/>
-      <c r="B26" s="110"/>
+      <c r="A26" s="122"/>
+      <c r="B26" s="122"/>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A27" s="110"/>
-      <c r="B27" s="110"/>
+      <c r="A27" s="122"/>
+      <c r="B27" s="122"/>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A28" s="110"/>
-      <c r="B28" s="110"/>
+      <c r="A28" s="122"/>
+      <c r="B28" s="122"/>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A29" s="110"/>
-      <c r="B29" s="110"/>
+      <c r="A29" s="122"/>
+      <c r="B29" s="122"/>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A30" s="110"/>
-      <c r="B30" s="110"/>
+      <c r="A30" s="122"/>
+      <c r="B30" s="122"/>
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="108"/>
+      <c r="B31" s="120"/>
       <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="110"/>
-      <c r="B32" s="110"/>
+      <c r="A32" s="122"/>
+      <c r="B32" s="122"/>
       <c r="C32" s="12"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="110"/>
-      <c r="B33" s="110"/>
+      <c r="A33" s="122"/>
+      <c r="B33" s="122"/>
       <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="110"/>
-      <c r="B34" s="110"/>
+      <c r="A34" s="122"/>
+      <c r="B34" s="122"/>
       <c r="C34" s="12"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="110"/>
-      <c r="B35" s="110"/>
+      <c r="A35" s="122"/>
+      <c r="B35" s="122"/>
       <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="110"/>
-      <c r="B36" s="110"/>
+      <c r="A36" s="122"/>
+      <c r="B36" s="122"/>
       <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="110"/>
-      <c r="B37" s="110"/>
+      <c r="A37" s="122"/>
+      <c r="B37" s="122"/>
       <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="110"/>
-      <c r="B38" s="110"/>
+      <c r="A38" s="122"/>
+      <c r="B38" s="122"/>
       <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="110"/>
-      <c r="B39" s="110"/>
+      <c r="A39" s="122"/>
+      <c r="B39" s="122"/>
       <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:9" s="13" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A40" s="108" t="s">
+      <c r="A40" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="108"/>
+      <c r="B40" s="120"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
@@ -3842,8 +3864,8 @@
       <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" s="13" customFormat="1">
-      <c r="A41" s="111"/>
-      <c r="B41" s="111"/>
+      <c r="A41" s="123"/>
+      <c r="B41" s="123"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
@@ -3853,8 +3875,8 @@
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" s="13" customFormat="1">
-      <c r="A42" s="111"/>
-      <c r="B42" s="111"/>
+      <c r="A42" s="123"/>
+      <c r="B42" s="123"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -3864,8 +3886,8 @@
       <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" s="13" customFormat="1">
-      <c r="A43" s="111"/>
-      <c r="B43" s="111"/>
+      <c r="A43" s="123"/>
+      <c r="B43" s="123"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -3875,8 +3897,8 @@
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" s="13" customFormat="1">
-      <c r="A44" s="111"/>
-      <c r="B44" s="111"/>
+      <c r="A44" s="123"/>
+      <c r="B44" s="123"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -3886,8 +3908,8 @@
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" s="13" customFormat="1">
-      <c r="A45" s="111"/>
-      <c r="B45" s="111"/>
+      <c r="A45" s="123"/>
+      <c r="B45" s="123"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
@@ -3896,8 +3918,8 @@
       <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" s="13" customFormat="1">
-      <c r="A46" s="111"/>
-      <c r="B46" s="111"/>
+      <c r="A46" s="123"/>
+      <c r="B46" s="123"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
@@ -3906,8 +3928,8 @@
       <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9" s="13" customFormat="1">
-      <c r="A47" s="111"/>
-      <c r="B47" s="111"/>
+      <c r="A47" s="123"/>
+      <c r="B47" s="123"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
@@ -3916,8 +3938,8 @@
       <c r="I47" s="12"/>
     </row>
     <row r="48" spans="1:9" s="13" customFormat="1">
-      <c r="A48" s="111"/>
-      <c r="B48" s="111"/>
+      <c r="A48" s="123"/>
+      <c r="B48" s="123"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
@@ -3926,10 +3948,10 @@
       <c r="I48" s="12"/>
     </row>
     <row r="49" spans="1:9" s="13" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A49" s="108" t="s">
+      <c r="A49" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="108"/>
+      <c r="B49" s="120"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
@@ -3938,8 +3960,8 @@
       <c r="I49" s="12"/>
     </row>
     <row r="50" spans="1:9" s="13" customFormat="1">
-      <c r="A50" s="109"/>
-      <c r="B50" s="109"/>
+      <c r="A50" s="121"/>
+      <c r="B50" s="121"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
@@ -3948,8 +3970,8 @@
       <c r="I50" s="12"/>
     </row>
     <row r="51" spans="1:9" s="13" customFormat="1">
-      <c r="A51" s="109"/>
-      <c r="B51" s="109"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="121"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
@@ -3958,8 +3980,8 @@
       <c r="I51" s="12"/>
     </row>
     <row r="52" spans="1:9" s="13" customFormat="1">
-      <c r="A52" s="109"/>
-      <c r="B52" s="109"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="121"/>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
@@ -3968,8 +3990,8 @@
       <c r="I52" s="12"/>
     </row>
     <row r="53" spans="1:9" s="13" customFormat="1">
-      <c r="A53" s="109"/>
-      <c r="B53" s="109"/>
+      <c r="A53" s="121"/>
+      <c r="B53" s="121"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
@@ -3978,8 +4000,8 @@
       <c r="I53" s="12"/>
     </row>
     <row r="54" spans="1:9" s="13" customFormat="1">
-      <c r="A54" s="109"/>
-      <c r="B54" s="109"/>
+      <c r="A54" s="121"/>
+      <c r="B54" s="121"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
@@ -3988,8 +4010,8 @@
       <c r="I54" s="12"/>
     </row>
     <row r="55" spans="1:9" s="13" customFormat="1">
-      <c r="A55" s="109"/>
-      <c r="B55" s="109"/>
+      <c r="A55" s="121"/>
+      <c r="B55" s="121"/>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
@@ -3998,8 +4020,8 @@
       <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:9" s="13" customFormat="1">
-      <c r="A56" s="109"/>
-      <c r="B56" s="109"/>
+      <c r="A56" s="121"/>
+      <c r="B56" s="121"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
@@ -4008,8 +4030,8 @@
       <c r="I56" s="12"/>
     </row>
     <row r="57" spans="1:9" s="13" customFormat="1">
-      <c r="A57" s="109"/>
-      <c r="B57" s="109"/>
+      <c r="A57" s="121"/>
+      <c r="B57" s="121"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
@@ -4019,6 +4041,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B57"/>
     <mergeCell ref="A22:B22"/>
@@ -4027,11 +4054,6 @@
     <mergeCell ref="A32:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B48"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
@@ -4053,14 +4075,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -4115,16 +4137,16 @@
       <c r="C2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="114" t="str">
+      <c r="D2" s="168" t="str">
         <f>IF('Identification projet'!B11="","Renseigner feuille Identification projet",'Identification projet'!B11)</f>
         <v>Renseigner feuille Identification projet</v>
       </c>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
       <c r="L2" s="79"/>
       <c r="M2" s="79"/>
       <c r="N2" s="80"/>
@@ -4148,16 +4170,16 @@
       <c r="C3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="114" t="str">
+      <c r="D3" s="168" t="str">
         <f>IF('Identification projet'!B12="","Renseigner feuille Identification projet",'Identification projet'!B12)</f>
         <v>Renseigner feuille Identification projet</v>
       </c>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
       <c r="K3" s="105"/>
       <c r="L3" s="84" t="s">
         <v>21</v>
@@ -4184,127 +4206,129 @@
       <c r="X3" s="83"/>
     </row>
     <row r="4" spans="1:29" ht="13.5" customHeight="1">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="169" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="166"/>
-      <c r="C4" s="165" t="s">
+      <c r="B4" s="170"/>
+      <c r="C4" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="150" t="s">
+      <c r="D4" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="151">
-        <v>0</v>
-      </c>
-      <c r="F4" s="151" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="151" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="152" t="s">
-        <v>28</v>
+      <c r="E4" s="108" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="108" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="109" t="s">
+        <v>87</v>
       </c>
       <c r="I4" s="96"/>
       <c r="K4" s="33" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="75" t="s">
+      <c r="R4" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="76" t="s">
+      <c r="S4" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="76" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="76" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="76" t="s">
+      <c r="T4" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="76" t="s">
+      <c r="U4" s="77" t="s">
         <v>33</v>
-      </c>
-      <c r="S4" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="77" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="77" t="s">
-        <v>36</v>
       </c>
       <c r="V4" s="77" t="s">
         <v>25</v>
       </c>
       <c r="W4" s="78" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="X4" s="78" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="13.5" customHeight="1">
-      <c r="A5" s="153" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="172"/>
+      <c r="A5" s="132" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="133"/>
       <c r="C5" s="99" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="176"/>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
-      <c r="H5" s="178"/>
+        <v>66</v>
+      </c>
+      <c r="D5" s="180"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="182"/>
       <c r="I5" s="96"/>
       <c r="K5" s="97">
         <v>0.2</v>
       </c>
       <c r="L5" s="74">
         <f>SUM(L6:L9)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P5" s="76">
         <f>SUM(P6:P9)</f>
-        <v>0</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="S5" s="75">
         <f>SUM(S6:S9)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T5" s="88">
         <f>IF(S5=0,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="78">
         <f>SUM(W6:W9)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X5" s="78">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="12.75" customHeight="1">
-      <c r="A6" s="154"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="155"/>
-      <c r="I6" s="36" t="str">
-        <f t="shared" ref="I6:I14" si="0">(IF(W6&lt;&gt;0,"◄",""))</f>
-        <v>◄</v>
+      <c r="A6" s="128"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="179" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="189"/>
+      <c r="E6" s="188" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="186"/>
+      <c r="G6" s="186"/>
+      <c r="H6" s="186"/>
+      <c r="I6" s="193" t="str">
+        <f>(IF(COUNTA($E$6:$H$9)&lt;&gt;1,"x",""))</f>
+        <v>x</v>
       </c>
       <c r="J6" s="37"/>
       <c r="K6" s="73">
@@ -4312,15 +4336,15 @@
         <v>1</v>
       </c>
       <c r="L6" s="85">
-        <f t="shared" ref="L6:L14" si="1">K6*S6</f>
-        <v>0</v>
+        <f t="shared" ref="L6:L14" si="0">K6*S6</f>
+        <v>1</v>
       </c>
       <c r="M6" s="76">
-        <f t="shared" ref="M6:M14" si="2">S6*K6*20</f>
-        <v>0</v>
+        <f t="shared" ref="M6:M14" si="1">S6*K6*20</f>
+        <v>20</v>
       </c>
       <c r="N6" s="76">
-        <f t="shared" ref="N6:N14" si="3">(IF(F6&lt;&gt;"",1/3,0)+IF(G6&lt;&gt;"",2/3,0)+IF(H6&lt;&gt;"",1,0))*K6*20</f>
+        <f t="shared" ref="N6:N14" si="2">(IF(F6&lt;&gt;"",1/3,0)+IF(G6&lt;&gt;"",2/3,0)+IF(H6&lt;&gt;"",1,0))*K6*20</f>
         <v>0</v>
       </c>
       <c r="O6" s="76" t="e">
@@ -4340,71 +4364,70 @@
         <v>#REF!</v>
       </c>
       <c r="S6" s="75">
-        <f t="shared" ref="S6:S14" si="4">IF(D6="",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
+        <f t="shared" ref="S6:S14" si="3">IF(D6="",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
+        <v>1</v>
       </c>
       <c r="T6" s="77">
-        <f t="shared" ref="T6:T14" si="5">IF(D6&lt;&gt;"",0,(IF(E6&lt;&gt;"",0.02,(N6/(K6*20)))))</f>
-        <v>0</v>
+        <f t="shared" ref="T6:T14" si="4">IF(D6&lt;&gt;"",0,(IF(E6&lt;&gt;"",0.02,(N6/(K6*20)))))</f>
+        <v>0.02</v>
       </c>
       <c r="U6" s="77">
-        <f t="shared" ref="U6:U14" si="6">IF(S6=0,0,K6)</f>
-        <v>0</v>
+        <f t="shared" ref="U6:U14" si="5">IF(S6=0,0,K6)</f>
+        <v>1</v>
       </c>
       <c r="V6" s="90">
-        <f t="shared" ref="V6:V14" si="7">IF(D6&lt;&gt;"",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="V6:V14" si="6">IF(D6&lt;&gt;"",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="W6" s="78">
-        <f t="shared" ref="W6:W14" si="8">IF(OR(S6&gt;1,V6&gt;0,AND(D6="",S6=0)),1,0)</f>
-        <v>1</v>
+        <f t="shared" ref="W6:W14" si="7">IF(OR(S6&gt;1,V6&gt;0,AND(D6="",S6=0)),1,0)</f>
+        <v>0</v>
       </c>
       <c r="X6" s="78" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="Y6" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:29">
-      <c r="A7" s="154"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="156"/>
-      <c r="I7" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>◄</v>
-      </c>
+      <c r="A7" s="128"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="179" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="190"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="188" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="186"/>
+      <c r="H7" s="186"/>
+      <c r="I7" s="193"/>
       <c r="J7" s="37"/>
       <c r="K7" s="73">
-        <f t="shared" ref="K7:K14" si="9">IF(D7="",1,0)</f>
+        <f t="shared" ref="K7:K14" si="8">IF(D7="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L7" s="85">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="76">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="76">
+        <v>20</v>
+      </c>
+      <c r="N7" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="76">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.6666666666666661</v>
       </c>
       <c r="O7" s="76" t="e">
         <f>IF(#REF!=0,0,M7/#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="P7" s="76">
-        <f t="shared" ref="P7:P9" si="10">IF($T$5=0,0,N7/$L$5)</f>
-        <v>0</v>
+        <f t="shared" ref="P7:P9" si="9">IF($T$5=0,0,N7/$L$5)</f>
+        <v>3.333333333333333</v>
       </c>
       <c r="Q7" s="76" t="e">
         <f>O7*#REF!</f>
@@ -4415,56 +4438,53 @@
         <v>#REF!</v>
       </c>
       <c r="S7" s="75">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="T7" s="77">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="77">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U7" s="77">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="77">
+        <v>1</v>
+      </c>
+      <c r="V7" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V7" s="90">
+      <c r="W7" s="78">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W7" s="78">
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="128"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="179" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="190"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="191"/>
+      <c r="G8" s="188"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="73">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="154"/>
-      <c r="B8" s="168"/>
-      <c r="C8" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="155"/>
-      <c r="I8" s="36" t="str">
+      <c r="L8" s="85">
         <f t="shared" si="0"/>
-        <v>◄</v>
-      </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="73">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L8" s="85">
+        <v>0</v>
+      </c>
+      <c r="M8" s="76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M8" s="76">
+      <c r="N8" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="76">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O8" s="76" t="e">
@@ -4472,7 +4492,7 @@
         <v>#REF!</v>
       </c>
       <c r="P8" s="76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q8" s="76" t="e">
@@ -4484,56 +4504,53 @@
         <v>#REF!</v>
       </c>
       <c r="S8" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T8" s="77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T8" s="77">
+      <c r="U8" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U8" s="77">
+      <c r="V8" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V8" s="90">
+      <c r="W8" s="78">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="134"/>
+      <c r="B9" s="135"/>
+      <c r="C9" s="179" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="190"/>
+      <c r="E9" s="192"/>
+      <c r="F9" s="192"/>
+      <c r="G9" s="191"/>
+      <c r="H9" s="187"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="73">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:29">
-      <c r="A9" s="173"/>
-      <c r="B9" s="174"/>
-      <c r="C9" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="156"/>
-      <c r="I9" s="36" t="str">
+      <c r="L9" s="85">
         <f t="shared" si="0"/>
-        <v>◄</v>
-      </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="73">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L9" s="85">
+        <v>0</v>
+      </c>
+      <c r="M9" s="76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M9" s="76">
+      <c r="N9" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="76">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O9" s="76" t="e">
@@ -4541,7 +4558,7 @@
         <v>#REF!</v>
       </c>
       <c r="P9" s="76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q9" s="76" t="e">
@@ -4553,41 +4570,41 @@
         <v>#REF!</v>
       </c>
       <c r="S9" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T9" s="77">
+      <c r="U9" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U9" s="77">
+      <c r="V9" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V9" s="90">
+      <c r="W9" s="78">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W9" s="78">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="170" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="171"/>
+      <c r="A10" s="126" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="127"/>
       <c r="C10" s="100" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="179"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="181"/>
+        <v>68</v>
+      </c>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="185"/>
       <c r="I10" s="36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J10" s="37"/>
       <c r="K10" s="97">
@@ -4620,35 +4637,35 @@
       </c>
     </row>
     <row r="11" spans="1:29" ht="12.75" customHeight="1">
-      <c r="A11" s="154"/>
-      <c r="B11" s="168"/>
+      <c r="A11" s="128"/>
+      <c r="B11" s="129"/>
       <c r="C11" s="35" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D11" s="41"/>
       <c r="E11" s="42"/>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
-      <c r="H11" s="155"/>
+      <c r="H11" s="110"/>
       <c r="I11" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I6:I14" si="10">(IF(W11&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J11" s="37"/>
       <c r="K11" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L11" s="85">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M11" s="76">
+      <c r="N11" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="76">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O11" s="76" t="e">
@@ -4668,56 +4685,56 @@
         <v>#REF!</v>
       </c>
       <c r="S11" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T11" s="77">
+      <c r="U11" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U11" s="77">
+      <c r="V11" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V11" s="90">
+      <c r="W11" s="78">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="78">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:29">
-      <c r="A12" s="154"/>
-      <c r="B12" s="168"/>
+      <c r="A12" s="128"/>
+      <c r="B12" s="129"/>
       <c r="C12" s="38" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
-      <c r="H12" s="156"/>
+      <c r="H12" s="111"/>
       <c r="I12" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>◄</v>
       </c>
       <c r="J12" s="37"/>
       <c r="K12" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L12" s="85">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M12" s="76">
+      <c r="N12" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="76">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O12" s="76" t="e">
@@ -4737,56 +4754,56 @@
         <v>#REF!</v>
       </c>
       <c r="S12" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T12" s="77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T12" s="77">
+      <c r="U12" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U12" s="77">
+      <c r="V12" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V12" s="90">
+      <c r="W12" s="78">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W12" s="78">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="13.5" customHeight="1">
-      <c r="A13" s="154"/>
-      <c r="B13" s="168"/>
+      <c r="A13" s="128"/>
+      <c r="B13" s="129"/>
       <c r="C13" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="42"/>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
-      <c r="H13" s="155"/>
+      <c r="H13" s="110"/>
       <c r="I13" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>◄</v>
       </c>
       <c r="J13" s="37"/>
       <c r="K13" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L13" s="85">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M13" s="76">
+      <c r="N13" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="76">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O13" s="76" t="e">
@@ -4806,56 +4823,56 @@
         <v>#REF!</v>
       </c>
       <c r="S13" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T13" s="77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T13" s="77">
+      <c r="U13" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U13" s="77">
+      <c r="V13" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V13" s="90">
+      <c r="W13" s="78">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W13" s="78">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="12.75" customHeight="1">
-      <c r="A14" s="157"/>
-      <c r="B14" s="169"/>
+      <c r="A14" s="130"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="40"/>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
-      <c r="H14" s="156"/>
+      <c r="H14" s="111"/>
       <c r="I14" s="36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>◄</v>
       </c>
       <c r="J14" s="37"/>
       <c r="K14" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L14" s="85">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="76">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M14" s="76">
+      <c r="N14" s="76">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="76">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14" s="76" t="e">
@@ -4875,44 +4892,44 @@
         <v>#REF!</v>
       </c>
       <c r="S14" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T14" s="77">
+      <c r="U14" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U14" s="77">
+      <c r="V14" s="90">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V14" s="90">
+      <c r="W14" s="78">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W14" s="78">
-        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Z14" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:29">
-      <c r="A15" s="153" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="172"/>
+      <c r="A15" s="132" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="133"/>
       <c r="C15" s="101" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="179"/>
-      <c r="E15" s="180"/>
-      <c r="F15" s="180"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="181"/>
+        <v>67</v>
+      </c>
+      <c r="D15" s="138"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="139"/>
+      <c r="H15" s="140"/>
       <c r="I15" s="36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="J15" s="37"/>
       <c r="K15" s="97">
@@ -4945,16 +4962,16 @@
       </c>
     </row>
     <row r="16" spans="1:29" ht="13.5" customHeight="1">
-      <c r="A16" s="154"/>
-      <c r="B16" s="168"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="129"/>
       <c r="C16" s="65" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D16" s="66"/>
       <c r="E16" s="67"/>
       <c r="F16" s="67"/>
       <c r="G16" s="68"/>
-      <c r="H16" s="158"/>
+      <c r="H16" s="112"/>
       <c r="I16" s="36" t="str">
         <f t="shared" ref="I16:I19" si="12">(IF(W16&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
@@ -5014,16 +5031,16 @@
       </c>
     </row>
     <row r="17" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A17" s="154"/>
-      <c r="B17" s="168"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="129"/>
       <c r="C17" s="38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D17" s="39"/>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
       <c r="G17" s="40"/>
-      <c r="H17" s="156"/>
+      <c r="H17" s="111"/>
       <c r="I17" s="36" t="str">
         <f t="shared" si="12"/>
         <v>◄</v>
@@ -5083,16 +5100,16 @@
       </c>
     </row>
     <row r="18" spans="1:30" ht="13.5" customHeight="1">
-      <c r="A18" s="154"/>
-      <c r="B18" s="168"/>
+      <c r="A18" s="128"/>
+      <c r="B18" s="129"/>
       <c r="C18" s="69" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D18" s="70"/>
       <c r="E18" s="71"/>
       <c r="F18" s="71"/>
       <c r="G18" s="72"/>
-      <c r="H18" s="159"/>
+      <c r="H18" s="113"/>
       <c r="I18" s="36" t="str">
         <f t="shared" si="12"/>
         <v>◄</v>
@@ -5152,16 +5169,16 @@
       </c>
     </row>
     <row r="19" spans="1:30" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A19" s="160"/>
-      <c r="B19" s="175"/>
-      <c r="C19" s="161" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="162"/>
-      <c r="E19" s="163"/>
-      <c r="F19" s="163"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="164"/>
+      <c r="A19" s="136"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="114" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="115"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="117"/>
       <c r="I19" s="36" t="str">
         <f t="shared" si="12"/>
         <v>◄</v>
@@ -5222,18 +5239,18 @@
     </row>
     <row r="20" spans="1:30" ht="17.850000000000001" customHeight="1">
       <c r="C20" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="112">
+        <v>65</v>
+      </c>
+      <c r="E20" s="148">
         <f>S5/X5</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="148"/>
+      <c r="G20" s="148"/>
+      <c r="H20" s="148"/>
       <c r="I20" s="36" t="str">
         <f t="shared" ref="I20:I23" si="23">(IF(E20&lt;0.5,"◄",""))</f>
-        <v>◄</v>
+        <v/>
       </c>
       <c r="K20" s="34">
         <f>K5+K10+K15</f>
@@ -5242,13 +5259,13 @@
       <c r="L20" s="91"/>
       <c r="S20" s="86">
         <f>S5+S10+S15</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U20" s="92"/>
       <c r="V20" s="93"/>
       <c r="W20" s="89">
         <f>W5+W10+W15</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X20" s="87">
         <f>X5+X10+X15</f>
@@ -5257,26 +5274,26 @@
     </row>
     <row r="21" spans="1:30" ht="17.850000000000001" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="112">
+        <v>63</v>
+      </c>
+      <c r="E21" s="148">
         <f>S10/X10</f>
         <v>0</v>
       </c>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="148"/>
+      <c r="H21" s="148"/>
       <c r="I21" s="36" t="str">
         <f t="shared" si="23"/>
         <v>◄</v>
       </c>
-      <c r="J21" s="113" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="113"/>
+      <c r="J21" s="171" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="171"/>
       <c r="L21" s="91"/>
       <c r="S21" s="87"/>
       <c r="U21" s="92"/>
@@ -5285,27 +5302,27 @@
     </row>
     <row r="22" spans="1:30" ht="17.850000000000001" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="112">
+        <v>64</v>
+      </c>
+      <c r="E22" s="148">
         <f>S15/X15</f>
         <v>0</v>
       </c>
-      <c r="F22" s="112"/>
-      <c r="G22" s="112"/>
-      <c r="H22" s="112"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="148"/>
+      <c r="H22" s="148"/>
       <c r="I22" s="36" t="str">
         <f t="shared" si="23"/>
         <v>◄</v>
       </c>
-      <c r="J22" s="113"/>
-      <c r="K22" s="113"/>
+      <c r="J22" s="171"/>
+      <c r="K22" s="171"/>
       <c r="L22" s="91"/>
       <c r="O22" s="76" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S22" s="87"/>
       <c r="U22" s="92"/>
@@ -5317,22 +5334,22 @@
     </row>
     <row r="23" spans="1:30" ht="17.850000000000001" customHeight="1">
       <c r="C23" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="112">
+        <v>69</v>
+      </c>
+      <c r="E23" s="148">
         <f>0.2*E20+0.4*E21+0.4*E22</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="112"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="112"/>
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="148"/>
+      <c r="G23" s="148"/>
+      <c r="H23" s="148"/>
       <c r="I23" s="36" t="str">
         <f t="shared" si="23"/>
         <v>◄</v>
       </c>
       <c r="K23" s="34"/>
       <c r="L23" s="91" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S23" s="87"/>
       <c r="U23" s="92"/>
@@ -5343,19 +5360,19 @@
       <c r="AD23" s="104"/>
     </row>
     <row r="24" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="C24" s="167" t="s">
-        <v>82</v>
+      <c r="C24" s="119" t="s">
+        <v>79</v>
       </c>
       <c r="D24" s="45"/>
-      <c r="E24" s="117" t="str">
+      <c r="E24" s="149" t="str">
         <f>IF(OR(E20&lt;0.5,E21&lt;0.5,E22&lt;0.5),"Tx&lt;50",IF(W20&lt;&gt;0,"Erreur",(IF(S20&lt;&gt;0,(P5*K5+P10*K10+P15*K15)/(T5*K5+T10*K10+T15*K15),0))))</f>
         <v>Tx&lt;50</v>
       </c>
-      <c r="F24" s="117"/>
-      <c r="G24" s="118" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="118"/>
+      <c r="F24" s="149"/>
+      <c r="G24" s="150" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="150"/>
       <c r="I24" s="46"/>
       <c r="R24" s="94"/>
       <c r="S24" s="94"/>
@@ -5365,89 +5382,89 @@
     </row>
     <row r="25" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
       <c r="C25" s="26" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D25" s="45"/>
-      <c r="E25" s="119"/>
-      <c r="F25" s="148"/>
-      <c r="G25" s="147" t="s">
+      <c r="E25" s="151"/>
+      <c r="F25" s="152"/>
+      <c r="G25" s="153" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="120"/>
+      <c r="H25" s="154"/>
       <c r="I25" s="48"/>
       <c r="AA25" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="18.75" customHeight="1" thickBot="1">
       <c r="C26" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="121" t="str">
+        <v>40</v>
+      </c>
+      <c r="E26" s="155" t="str">
         <f>IF(W20&lt;&gt;0,"",E25*'Identification projet'!B5)</f>
         <v/>
       </c>
-      <c r="F26" s="146"/>
-      <c r="G26" s="145">
+      <c r="F26" s="156"/>
+      <c r="G26" s="157">
         <f>(20*'Identification projet'!B5)</f>
         <v>100</v>
       </c>
-      <c r="H26" s="122"/>
+      <c r="H26" s="158"/>
       <c r="I26" s="36"/>
       <c r="J26" s="50"/>
     </row>
     <row r="27" spans="1:30" ht="14.1" customHeight="1">
-      <c r="A27" s="123" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
+      <c r="A27" s="159" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="159"/>
+      <c r="C27" s="159"/>
+      <c r="D27" s="159"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="159"/>
+      <c r="G27" s="159"/>
+      <c r="H27" s="159"/>
       <c r="I27" s="48"/>
       <c r="J27" s="50"/>
     </row>
     <row r="28" spans="1:30" ht="14.1" customHeight="1" thickBot="1">
       <c r="A28" s="51"/>
       <c r="B28" s="51"/>
-      <c r="C28" s="144" t="str">
+      <c r="C28" s="160" t="str">
         <f>(IF(W20&gt;0,"ATTENTION. Erreur de saisie : cocher une seule colonne par ligne ! Voir repères ◄ à droite de la grille.",""))</f>
         <v>ATTENTION. Erreur de saisie : cocher une seule colonne par ligne ! Voir repères ◄ à droite de la grille.</v>
       </c>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="144"/>
-      <c r="G28" s="144"/>
-      <c r="H28" s="144"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="160"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="160"/>
       <c r="I28" s="47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="15" customHeight="1">
-      <c r="A29" s="124" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="143"/>
-      <c r="C29" s="142"/>
-      <c r="D29" s="142"/>
-      <c r="E29" s="142"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="142"/>
-      <c r="H29" s="125"/>
+      <c r="A29" s="161" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="162"/>
+      <c r="C29" s="163"/>
+      <c r="D29" s="163"/>
+      <c r="E29" s="163"/>
+      <c r="F29" s="163"/>
+      <c r="G29" s="163"/>
+      <c r="H29" s="164"/>
       <c r="I29" s="52"/>
     </row>
     <row r="30" spans="1:30" ht="84.75" customHeight="1" thickBot="1">
-      <c r="A30" s="139"/>
-      <c r="B30" s="140"/>
-      <c r="C30" s="140"/>
-      <c r="D30" s="140"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="140"/>
-      <c r="G30" s="140"/>
-      <c r="H30" s="141"/>
+      <c r="A30" s="165"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="166"/>
+      <c r="D30" s="166"/>
+      <c r="E30" s="166"/>
+      <c r="F30" s="166"/>
+      <c r="G30" s="166"/>
+      <c r="H30" s="167"/>
       <c r="I30" s="53"/>
     </row>
     <row r="31" spans="1:30" ht="7.5" customHeight="1" thickBot="1">
@@ -5462,72 +5479,72 @@
       <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="146" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="146"/>
+      <c r="C32" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="58"/>
+      <c r="E32" s="147" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
+      <c r="H32" s="147"/>
+      <c r="I32" s="59"/>
+    </row>
+    <row r="33" spans="1:9" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="143"/>
+      <c r="B33" s="143"/>
+      <c r="C33" s="60"/>
+      <c r="E33" s="144"/>
+      <c r="F33" s="144"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="61"/>
+    </row>
+    <row r="34" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A34" s="143"/>
+      <c r="B34" s="143"/>
+      <c r="C34" s="60"/>
+    </row>
+    <row r="35" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A35" s="145"/>
+      <c r="B35" s="145"/>
+      <c r="C35" s="60"/>
+    </row>
+    <row r="36" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A36" s="143"/>
+      <c r="B36" s="143"/>
+      <c r="C36" s="60"/>
+    </row>
+    <row r="37" spans="1:9" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A37" s="141"/>
+      <c r="B37" s="141"/>
+      <c r="C37" s="62"/>
+      <c r="E37" s="142">
+        <v>41739</v>
+      </c>
+      <c r="F37" s="142"/>
+      <c r="G37" s="142"/>
+      <c r="H37" s="142"/>
+      <c r="I37" s="64" t="s">
         <v>46</v>
-      </c>
-      <c r="B32" s="115"/>
-      <c r="C32" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="58"/>
-      <c r="E32" s="116" t="s">
-        <v>48</v>
-      </c>
-      <c r="F32" s="116"/>
-      <c r="G32" s="116"/>
-      <c r="H32" s="116"/>
-      <c r="I32" s="59"/>
-    </row>
-    <row r="33" spans="1:9" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="128"/>
-      <c r="B33" s="128"/>
-      <c r="C33" s="60"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="61"/>
-    </row>
-    <row r="34" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A34" s="128"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="60"/>
-    </row>
-    <row r="35" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A35" s="130"/>
-      <c r="B35" s="130"/>
-      <c r="C35" s="60"/>
-    </row>
-    <row r="36" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A36" s="128"/>
-      <c r="B36" s="128"/>
-      <c r="C36" s="60"/>
-    </row>
-    <row r="37" spans="1:9" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A37" s="126"/>
-      <c r="B37" s="126"/>
-      <c r="C37" s="62"/>
-      <c r="E37" s="127">
-        <v>41739</v>
-      </c>
-      <c r="F37" s="127"/>
-      <c r="G37" s="127"/>
-      <c r="H37" s="127"/>
-      <c r="I37" s="64" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="14.25">
       <c r="A39" s="14">
         <f>W20</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" s="63"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="98">
         <f>W5</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -5557,24 +5574,19 @@
     <row r="45" spans="1:9">
       <c r="A45" s="14">
         <f>W6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A10:B14"/>
-    <mergeCell ref="A5:B9"/>
-    <mergeCell ref="A15:B19"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
+  <mergeCells count="35">
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="J21:K22"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="I6:I9"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="E23:H23"/>
@@ -5589,14 +5601,25 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:H29"/>
     <mergeCell ref="A30:H30"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="J21:K22"/>
-    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A10:B14"/>
+    <mergeCell ref="A5:B9"/>
+    <mergeCell ref="A15:B19"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D15:H15"/>
   </mergeCells>
+  <conditionalFormatting sqref="I6:I9">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.27569444444444446" right="0.19652777777777777" top="0.12986111111111112" bottom="0.15763888888888888" header="0.51180555555555551" footer="0.15763888888888888"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -5613,7 +5636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D6:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5627,114 +5650,114 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:7">
-      <c r="D6" s="131"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="131"/>
-      <c r="G6" s="132"/>
+      <c r="D6" s="172"/>
+      <c r="E6" s="174"/>
+      <c r="F6" s="172"/>
+      <c r="G6" s="174"/>
     </row>
     <row r="7" spans="4:7">
-      <c r="D7" s="131"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="132"/>
+      <c r="D7" s="172"/>
+      <c r="E7" s="173"/>
+      <c r="F7" s="173"/>
+      <c r="G7" s="174"/>
     </row>
     <row r="8" spans="4:7" ht="24" customHeight="1">
-      <c r="D8" s="134" t="s">
+      <c r="D8" s="177" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="177" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="177" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="177" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7">
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="178"/>
+      <c r="G9" s="178"/>
+    </row>
+    <row r="10" spans="4:7" ht="60" customHeight="1">
+      <c r="D10" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="177" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="134" t="s">
+      <c r="F10" s="177" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="177" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7">
+      <c r="D11" s="178"/>
+      <c r="E11" s="178"/>
+      <c r="F11" s="178"/>
+      <c r="G11" s="178"/>
+    </row>
+    <row r="12" spans="4:7" ht="36" customHeight="1">
+      <c r="D12" s="177" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="134" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="134" t="s">
+      <c r="E12" s="177" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="177" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="4:7">
-      <c r="D9" s="135"/>
-      <c r="E9" s="135"/>
-      <c r="F9" s="135"/>
-      <c r="G9" s="135"/>
-    </row>
-    <row r="10" spans="4:7" ht="60" customHeight="1">
-      <c r="D10" s="134" t="s">
+      <c r="G12" s="177" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="134" t="s">
+    </row>
+    <row r="13" spans="4:7">
+      <c r="D13" s="178"/>
+      <c r="E13" s="178"/>
+      <c r="F13" s="178"/>
+      <c r="G13" s="178"/>
+    </row>
+    <row r="14" spans="4:7" ht="60" customHeight="1">
+      <c r="D14" s="175"/>
+      <c r="E14" s="175"/>
+      <c r="F14" s="177" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="134" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="134" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="4:7">
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-    </row>
-    <row r="12" spans="4:7" ht="36" customHeight="1">
-      <c r="D12" s="134" t="s">
+      <c r="G14" s="177" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="134" t="s">
+    </row>
+    <row r="15" spans="4:7">
+      <c r="D15" s="176"/>
+      <c r="E15" s="176"/>
+      <c r="F15" s="178"/>
+      <c r="G15" s="178"/>
+    </row>
+    <row r="16" spans="4:7" ht="60" customHeight="1">
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="177" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="134" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="134" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7">
-      <c r="D13" s="135"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="135"/>
-    </row>
-    <row r="14" spans="4:7" ht="60" customHeight="1">
-      <c r="D14" s="136"/>
-      <c r="E14" s="136"/>
-      <c r="F14" s="134" t="s">
+      <c r="G16" s="177" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="134" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7">
-      <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="135"/>
-    </row>
-    <row r="16" spans="4:7" ht="60" customHeight="1">
-      <c r="D16" s="136"/>
-      <c r="E16" s="136"/>
-      <c r="F16" s="134" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="134" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="17" spans="4:7">
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="135"/>
-      <c r="G17" s="135"/>
+      <c r="D17" s="176"/>
+      <c r="E17" s="176"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="178"/>
     </row>
     <row r="18" spans="4:7">
-      <c r="D18" s="131"/>
-      <c r="E18" s="133"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="132"/>
+      <c r="D18" s="172"/>
+      <c r="E18" s="173"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="174"/>
     </row>
     <row r="19" spans="4:7">
       <c r="D19" s="95"/>
@@ -5774,6 +5797,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
@@ -5783,21 +5821,6 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>